<commit_message>
Informacion dinamica en las actas
</commit_message>
<xml_diff>
--- a/php/report/plantilla_acta_donacion.xlsx
+++ b/php/report/plantilla_acta_donacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\InventarioISTGTest\php\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{577DB2D1-7C0D-4627-B0DC-89EBDD7AB4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCE38C9-7A34-449A-A119-148DBF06DCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>ENTREGUE CONFORME</t>
   </si>
@@ -37,18 +37,6 @@
     <t>OBSERVACIONES</t>
   </si>
   <si>
-    <t>&lt;nombre de quien entrega&gt;</t>
-  </si>
-  <si>
-    <t>&lt;nombre de quien recibe&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C.C. </t>
-  </si>
-  <si>
-    <t>C.C.</t>
-  </si>
-  <si>
     <t xml:space="preserve">AREA: </t>
   </si>
   <si>
@@ -59,12 +47,6 @@
   </si>
   <si>
     <t>ACTA DE DONACION</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En la ciudad de Guayaquil, Provincia de Guayas a los ______ días del mes de _____ de _____, en las oficinas del ISTG, ubicadas _______________________________ se reúnen por una parte_______________________, en calidad de Rectora, y  por otra parte ______________________ en calidad de  donante . </t>
-  </si>
-  <si>
-    <t xml:space="preserve">__________________________ realizará la donación de bienes muebles al Instituto Superior Tecnológico Guayaquil, los mismos que se detallan a continuación.  </t>
   </si>
   <si>
     <t xml:space="preserve">observacion </t>
@@ -700,7 +682,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -779,26 +761,50 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -809,40 +815,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1238,8 +1211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1273,18 +1246,18 @@
       <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" ht="27" x14ac:dyDescent="0.4">
-      <c r="A6" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="46"/>
+      <c r="A6" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="1:10" ht="27" x14ac:dyDescent="0.4">
       <c r="A7" s="16"/>
@@ -1295,42 +1268,38 @@
       <c r="F7" s="17"/>
       <c r="G7" s="17"/>
       <c r="H7" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="I7" s="17"/>
       <c r="J7" s="18"/>
     </row>
     <row r="8" spans="1:10" ht="102" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="51"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="52"/>
+      <c r="A8" s="43"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="45"/>
     </row>
     <row r="9" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A9" s="19"/>
       <c r="J9" s="20"/>
     </row>
     <row r="10" spans="1:10" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="53" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="54"/>
-      <c r="C10" s="54"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="54"/>
-      <c r="F10" s="54"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="54"/>
-      <c r="I10" s="54"/>
-      <c r="J10" s="55"/>
+      <c r="A10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
+      <c r="J10" s="48"/>
     </row>
     <row r="11" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A11" s="19"/>
@@ -1339,22 +1308,22 @@
     <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A12" s="26"/>
       <c r="B12" s="6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>4</v>
@@ -1365,7 +1334,7 @@
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="27"/>
       <c r="B13" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -1378,17 +1347,17 @@
     </row>
     <row r="14" spans="1:10" ht="92.25" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="48"/>
-      <c r="J14" s="49"/>
+        <v>9</v>
+      </c>
+      <c r="B14" s="41"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="42"/>
     </row>
     <row r="15" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A15" s="19"/>
@@ -1399,18 +1368,18 @@
       <c r="J16" s="20"/>
     </row>
     <row r="17" spans="1:10" ht="84" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="41" t="s">
+      <c r="A17" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="43"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="50"/>
+      <c r="H17" s="50"/>
+      <c r="I17" s="50"/>
+      <c r="J17" s="51"/>
     </row>
     <row r="18" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A18" s="19"/>
@@ -1439,15 +1408,15 @@
       <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="32"/>
+      <c r="B24" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="G24" s="39" t="s">
+      <c r="G24" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="H24" s="39"/>
+      <c r="H24" s="52"/>
       <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.4">
@@ -1471,51 +1440,43 @@
       <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A28" s="33" t="s">
+      <c r="A28" s="33"/>
+      <c r="B28" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="47"/>
-      <c r="C28" s="47"/>
-      <c r="G28" s="56" t="s">
+      <c r="C28" s="33"/>
+      <c r="G28" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="H28" s="56"/>
+      <c r="H28" s="53"/>
       <c r="J28" s="20"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A29" s="35" t="s">
+      <c r="A29" s="34"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="G29" s="39"/>
+      <c r="H29" s="39"/>
+      <c r="J29" s="20"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A30" s="34"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="G30" s="39"/>
+      <c r="H30" s="39"/>
+      <c r="J30" s="20"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A31" s="35"/>
+      <c r="B31" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="36"/>
-      <c r="C29" s="36"/>
-      <c r="G29" s="40" t="s">
+      <c r="C31" s="35"/>
+      <c r="G31" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="H29" s="40"/>
-      <c r="J29" s="20"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A30" s="35" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="47"/>
-      <c r="C30" s="47"/>
-      <c r="G30" s="40" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" s="40"/>
-      <c r="J30" s="20"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A31" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="34"/>
-      <c r="C31" s="31"/>
-      <c r="G31" s="38" t="s">
-        <v>10</v>
-      </c>
-      <c r="H31" s="38"/>
+      <c r="H31" s="40"/>
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.4">
@@ -1541,10 +1502,9 @@
       <c r="J34" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="10">
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="G29:H29"/>
-    <mergeCell ref="B30:C30"/>
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="B14:J14"/>
@@ -1552,7 +1512,6 @@
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="A17:J17"/>
     <mergeCell ref="G24:H24"/>
-    <mergeCell ref="B28:C28"/>
     <mergeCell ref="G28:H28"/>
   </mergeCells>
   <conditionalFormatting sqref="A13">

</xml_diff>